<commit_message>
added one slightly bigger test for the fun of it
yolo
</commit_message>
<xml_diff>
--- a/Tests.xlsx
+++ b/Tests.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\Uni\5a\1s\MEI\Exercicios\mei-assignment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\Uni\5a\1s\MEI\Exercicios\mei-assignment\MEI-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3DB2D18-138D-4C6B-8891-CDA685ADC35F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21354C33-9C32-45DD-A894-5AF35DE5F586}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3135" yWindow="3075" windowWidth="21600" windowHeight="11295" xr2:uid="{0DA2E7A0-E47A-415A-B459-0855BCC44AE6}"/>
   </bookViews>

</xml_diff>